<commit_message>
update plan2: add some contents in 3
</commit_message>
<xml_diff>
--- a/drafts/网络舆情量化分析论文数据.xlsx
+++ b/drafts/网络舆情量化分析论文数据.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_tiny-boat\ktsq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_tiny-boat\tiny-boat.github.io\drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9762" uniqueCount="6926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9764" uniqueCount="6928">
   <si>
     <t>爬取时间(__time)</t>
   </si>
@@ -34927,6 +34927,14 @@
       </rPr>
       <t>实验结果证明本文所用算法是有效的。</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文章意义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无意义</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -35038,7 +35046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -35083,6 +35091,8 @@
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -35387,10 +35397,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35408,7 +35419,9 @@
       <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="44" t="s">
+        <v>6926</v>
+      </c>
       <c r="D1" s="5" t="s">
         <v>430</v>
       </c>
@@ -35422,7 +35435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3304</v>
       </c>
@@ -35443,7 +35456,7 @@
         <v>3306</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3304</v>
       </c>
@@ -35464,7 +35477,7 @@
         <v>3372</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3304</v>
       </c>
@@ -35485,7 +35498,7 @@
         <v>3450</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3304</v>
       </c>
@@ -35506,7 +35519,7 @@
         <v>3462</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3269</v>
       </c>
@@ -35527,7 +35540,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3273</v>
       </c>
@@ -35555,7 +35568,9 @@
       <c r="B8" s="26" t="s">
         <v>3386</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="45" t="s">
+        <v>6927</v>
+      </c>
       <c r="D8" s="36" t="s">
         <v>6640</v>
       </c>
@@ -35569,7 +35584,7 @@
         <v>3388</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3278</v>
       </c>
@@ -35590,7 +35605,7 @@
         <v>3280</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>3366</v>
       </c>
@@ -35611,7 +35626,7 @@
         <v>3368</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3250</v>
       </c>
@@ -35632,7 +35647,7 @@
         <v>3252</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>168</v>
       </c>
@@ -35653,7 +35668,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3435</v>
       </c>
@@ -35674,7 +35689,7 @@
         <v>3437</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -35716,7 +35731,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>116</v>
       </c>
@@ -35758,7 +35773,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -35779,7 +35794,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -35800,7 +35815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3410</v>
       </c>
@@ -35821,7 +35836,7 @@
         <v>3412</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>3215</v>
       </c>
@@ -35842,7 +35857,7 @@
         <v>3217</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>3215</v>
       </c>
@@ -35863,7 +35878,7 @@
         <v>3331</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>107</v>
       </c>
@@ -35884,7 +35899,7 @@
         <v>3196</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>107</v>
       </c>
@@ -35905,7 +35920,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>418</v>
       </c>
@@ -35926,7 +35941,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>134</v>
       </c>
@@ -35947,7 +35962,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>134</v>
       </c>
@@ -35968,7 +35983,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>3465</v>
       </c>
@@ -35989,7 +36004,7 @@
         <v>3467</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>175</v>
       </c>
@@ -36031,7 +36046,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>40</v>
       </c>
@@ -36052,7 +36067,7 @@
         <v>3212</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -36073,7 +36088,7 @@
         <v>3476</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>3236</v>
       </c>
@@ -36094,7 +36109,7 @@
         <v>3238</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>125</v>
       </c>
@@ -36115,7 +36130,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>3206</v>
       </c>
@@ -36157,7 +36172,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>401</v>
       </c>
@@ -36220,7 +36235,7 @@
         <v>3472</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>23</v>
       </c>
@@ -36241,7 +36256,7 @@
         <v>3228</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>537</v>
       </c>
@@ -36262,7 +36277,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>537</v>
       </c>
@@ -36283,7 +36298,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>558</v>
       </c>
@@ -36304,7 +36319,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>558</v>
       </c>
@@ -36325,7 +36340,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>558</v>
       </c>
@@ -36346,7 +36361,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>570</v>
       </c>
@@ -36367,7 +36382,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>570</v>
       </c>
@@ -36388,7 +36403,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>626</v>
       </c>
@@ -36409,7 +36424,7 @@
         <v>6553</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>668</v>
       </c>
@@ -36430,7 +36445,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>677</v>
       </c>
@@ -36451,7 +36466,7 @@
         <v>6416</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6249</v>
       </c>
@@ -36472,7 +36487,7 @@
         <v>6776</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>6249</v>
       </c>
@@ -36493,7 +36508,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>6249</v>
       </c>
@@ -36514,7 +36529,7 @@
         <v>6282</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>6249</v>
       </c>
@@ -36535,7 +36550,7 @@
         <v>6286</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>699</v>
       </c>
@@ -36556,7 +36571,7 @@
         <v>6484</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>5956</v>
       </c>
@@ -36577,7 +36592,7 @@
         <v>5958</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>5956</v>
       </c>
@@ -36598,7 +36613,7 @@
         <v>6270</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>5589</v>
       </c>
@@ -36619,7 +36634,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>5589</v>
       </c>
@@ -36640,7 +36655,7 @@
         <v>6502</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>6257</v>
       </c>
@@ -36661,7 +36676,7 @@
         <v>6259</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>6257</v>
       </c>
@@ -36682,7 +36697,7 @@
         <v>6278</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>6007</v>
       </c>
@@ -36703,7 +36718,7 @@
         <v>6009</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>6007</v>
       </c>
@@ -36724,7 +36739,7 @@
         <v>6202</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>716</v>
       </c>
@@ -36745,7 +36760,7 @@
         <v>6179</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>5918</v>
       </c>
@@ -36766,7 +36781,7 @@
         <v>5920</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>5498</v>
       </c>
@@ -36787,7 +36802,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>5539</v>
       </c>
@@ -36808,7 +36823,7 @@
         <v>5996</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>5539</v>
       </c>
@@ -36829,7 +36844,7 @@
         <v>6195</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>5178</v>
       </c>
@@ -36850,7 +36865,7 @@
         <v>5533</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>5178</v>
       </c>
@@ -36871,7 +36886,7 @@
         <v>5742</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>5178</v>
       </c>
@@ -36892,7 +36907,7 @@
         <v>5746</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>5178</v>
       </c>
@@ -36913,7 +36928,7 @@
         <v>5911</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>5509</v>
       </c>
@@ -36934,7 +36949,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>5646</v>
       </c>
@@ -36955,7 +36970,7 @@
         <v>5648</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>6252</v>
       </c>
@@ -36976,7 +36991,7 @@
         <v>6254</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
         <v>5276</v>
       </c>
@@ -36997,7 +37012,7 @@
         <v>5278</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>5465</v>
       </c>
@@ -37018,7 +37033,7 @@
         <v>5467</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
         <v>5163</v>
       </c>
@@ -37039,7 +37054,7 @@
         <v>5487</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>5150</v>
       </c>
@@ -37060,7 +37075,7 @@
         <v>5152</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
         <v>5150</v>
       </c>
@@ -37081,7 +37096,7 @@
         <v>5495</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>5150</v>
       </c>
@@ -37102,7 +37117,7 @@
         <v>5641</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>5913</v>
       </c>
@@ -37123,7 +37138,7 @@
         <v>5915</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>5651</v>
       </c>
@@ -37144,7 +37159,7 @@
         <v>5617</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>5112</v>
       </c>
@@ -37165,7 +37180,7 @@
         <v>5458</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>5168</v>
       </c>
@@ -37186,7 +37201,7 @@
         <v>5388</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>5168</v>
       </c>
@@ -37207,7 +37222,7 @@
         <v>5392</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>725</v>
       </c>
@@ -37228,7 +37243,7 @@
         <v>5144</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>725</v>
       </c>
@@ -37249,7 +37264,7 @@
         <v>5430</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
         <v>725</v>
       </c>
@@ -37270,7 +37285,7 @@
         <v>5462</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>5096</v>
       </c>
@@ -37333,7 +37348,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>4833</v>
       </c>
@@ -37354,7 +37369,7 @@
         <v>4837</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>4709</v>
       </c>
@@ -37375,7 +37390,7 @@
         <v>4711</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>4709</v>
       </c>
@@ -37396,7 +37411,7 @@
         <v>4951</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>4812</v>
       </c>
@@ -37417,7 +37432,7 @@
         <v>4944</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
         <v>4958</v>
       </c>
@@ -37438,7 +37453,7 @@
         <v>4960</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>5056</v>
       </c>
@@ -37459,7 +37474,7 @@
         <v>5058</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>5056</v>
       </c>
@@ -37480,7 +37495,7 @@
         <v>5207</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>5056</v>
       </c>
@@ -37501,7 +37516,7 @@
         <v>5219</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>5056</v>
       </c>
@@ -37543,7 +37558,7 @@
         <v>4694</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>4527</v>
       </c>
@@ -37564,7 +37579,7 @@
         <v>4529</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="17" t="s">
         <v>4894</v>
       </c>
@@ -37585,7 +37600,7 @@
         <v>4895</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>4637</v>
       </c>
@@ -37606,7 +37621,7 @@
         <v>4899</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>4637</v>
       </c>
@@ -37627,7 +37642,7 @@
         <v>5147</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="17" t="s">
         <v>5714</v>
       </c>
@@ -37648,7 +37663,7 @@
         <v>5716</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>4272</v>
       </c>
@@ -37669,7 +37684,7 @@
         <v>4426</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>4347</v>
       </c>
@@ -37690,7 +37705,7 @@
         <v>4488</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>4347</v>
       </c>
@@ -37711,7 +37726,7 @@
         <v>4514</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>4347</v>
       </c>
@@ -37732,7 +37747,7 @@
         <v>4605</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>4347</v>
       </c>
@@ -37753,7 +37768,7 @@
         <v>4972</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>4556</v>
       </c>
@@ -37774,7 +37789,7 @@
         <v>4558</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>6429</v>
       </c>
@@ -37837,7 +37852,7 @@
         <v>4414</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>4328</v>
       </c>
@@ -37879,7 +37894,7 @@
         <v>4471</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>3733</v>
       </c>
@@ -37900,7 +37915,7 @@
         <v>4211</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>3733</v>
       </c>
@@ -37921,7 +37936,7 @@
         <v>4715</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>4104</v>
       </c>
@@ -37942,7 +37957,7 @@
         <v>4932</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>3653</v>
       </c>
@@ -37963,7 +37978,7 @@
         <v>3655</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>4097</v>
       </c>
@@ -37984,7 +37999,7 @@
         <v>4484</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>4657</v>
       </c>
@@ -38005,7 +38020,7 @@
         <v>4659</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>4123</v>
       </c>
@@ -38026,7 +38041,7 @@
         <v>4173</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
         <v>3706</v>
       </c>
@@ -38047,7 +38062,7 @@
         <v>4169</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>3706</v>
       </c>
@@ -38068,7 +38083,7 @@
         <v>4337</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>3706</v>
       </c>
@@ -38089,7 +38104,7 @@
         <v>6062</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>4217</v>
       </c>
@@ -38110,7 +38125,7 @@
         <v>4219</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>4028</v>
       </c>
@@ -38131,7 +38146,7 @@
         <v>4030</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="17" t="s">
         <v>3728</v>
       </c>
@@ -38152,7 +38167,7 @@
         <v>3974</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>3728</v>
       </c>
@@ -38173,7 +38188,7 @@
         <v>3978</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>3728</v>
       </c>
@@ -38194,7 +38209,7 @@
         <v>4045</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>3658</v>
       </c>
@@ -38215,7 +38230,7 @@
         <v>3660</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>3819</v>
       </c>
@@ -38236,7 +38251,7 @@
         <v>5788</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>3523</v>
       </c>
@@ -38257,7 +38272,7 @@
         <v>4034</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>3528</v>
       </c>
@@ -38278,7 +38293,7 @@
         <v>3530</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>3528</v>
       </c>
@@ -38299,7 +38314,7 @@
         <v>3581</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>3528</v>
       </c>
@@ -38320,7 +38335,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>3528</v>
       </c>
@@ -38341,7 +38356,7 @@
         <v>3986</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>3528</v>
       </c>
@@ -38383,7 +38398,7 @@
         <v>3959</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>3957</v>
       </c>
@@ -38404,7 +38419,7 @@
         <v>3963</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>734</v>
       </c>
@@ -38446,7 +38461,7 @@
         <v>3641</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>734</v>
       </c>
@@ -38467,7 +38482,7 @@
         <v>4207</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>3989</v>
       </c>
@@ -38488,7 +38503,7 @@
         <v>3991</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>3644</v>
       </c>
@@ -38509,7 +38524,7 @@
         <v>4360</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>3584</v>
       </c>
@@ -38530,7 +38545,7 @@
         <v>4226</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>739</v>
       </c>
@@ -38551,7 +38566,7 @@
         <v>4437</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>744</v>
       </c>
@@ -38572,7 +38587,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>769</v>
       </c>
@@ -38593,7 +38608,7 @@
         <v>3982</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>769</v>
       </c>
@@ -38614,7 +38629,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>769</v>
       </c>
@@ -38635,7 +38650,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="17" t="s">
         <v>4128</v>
       </c>
@@ -38656,7 +38671,7 @@
         <v>4130</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>3588</v>
       </c>
@@ -38677,7 +38692,7 @@
         <v>3589</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>3588</v>
       </c>
@@ -38698,7 +38713,7 @@
         <v>4390</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>803</v>
       </c>
@@ -38719,7 +38734,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>3604</v>
       </c>
@@ -38740,7 +38755,7 @@
         <v>3606</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>825</v>
       </c>
@@ -38761,7 +38776,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>306</v>
       </c>
@@ -38782,7 +38797,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>893</v>
       </c>
@@ -38803,7 +38818,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="17" t="s">
         <v>926</v>
       </c>
@@ -38824,7 +38839,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>939</v>
       </c>
@@ -38845,7 +38860,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>939</v>
       </c>
@@ -38866,7 +38881,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>1002</v>
       </c>
@@ -38887,7 +38902,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>1023</v>
       </c>
@@ -38908,7 +38923,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>1028</v>
       </c>
@@ -38929,7 +38944,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>1054</v>
       </c>
@@ -38950,7 +38965,7 @@
         <v>3480</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>1054</v>
       </c>
@@ -38971,7 +38986,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>6244</v>
       </c>
@@ -38992,7 +39007,7 @@
         <v>6246</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="17" t="s">
         <v>222</v>
       </c>
@@ -39013,7 +39028,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="17" t="s">
         <v>1122</v>
       </c>
@@ -39034,7 +39049,7 @@
         <v>3492</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>1122</v>
       </c>
@@ -39055,7 +39070,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>1122</v>
       </c>
@@ -39076,7 +39091,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>1171</v>
       </c>
@@ -39097,7 +39112,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>1176</v>
       </c>
@@ -39118,7 +39133,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>1231</v>
       </c>
@@ -39139,7 +39154,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>1263</v>
       </c>
@@ -39160,7 +39175,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>1263</v>
       </c>
@@ -39181,7 +39196,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>247</v>
       </c>
@@ -39202,7 +39217,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>247</v>
       </c>
@@ -39223,7 +39238,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
         <v>247</v>
       </c>
@@ -39244,7 +39259,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>1363</v>
       </c>
@@ -39265,7 +39280,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>1394</v>
       </c>
@@ -39286,7 +39301,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>1499</v>
       </c>
@@ -39307,7 +39322,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="17" t="s">
         <v>6496</v>
       </c>
@@ -39328,7 +39343,7 @@
         <v>6498</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>1668</v>
       </c>
@@ -39349,7 +39364,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="17" t="s">
         <v>1697</v>
       </c>
@@ -39370,7 +39385,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>252</v>
       </c>
@@ -39391,7 +39406,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>1814</v>
       </c>
@@ -39412,7 +39427,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>1848</v>
       </c>
@@ -39433,7 +39448,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>1853</v>
       </c>
@@ -39454,7 +39469,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>1953</v>
       </c>
@@ -39475,7 +39490,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="17" t="s">
         <v>1953</v>
       </c>
@@ -39496,7 +39511,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>1953</v>
       </c>
@@ -39517,7 +39532,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="17" t="s">
         <v>1953</v>
       </c>
@@ -39538,7 +39553,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="17" t="s">
         <v>2016</v>
       </c>
@@ -39559,7 +39574,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>2016</v>
       </c>
@@ -39580,7 +39595,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="17" t="s">
         <v>2102</v>
       </c>
@@ -39622,7 +39637,7 @@
         <v>4230</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>2116</v>
       </c>
@@ -39643,7 +39658,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="17" t="s">
         <v>2116</v>
       </c>
@@ -39664,7 +39679,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>2261</v>
       </c>
@@ -39706,7 +39721,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="17" t="s">
         <v>207</v>
       </c>
@@ -39727,7 +39742,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>207</v>
       </c>
@@ -39748,7 +39763,7 @@
         <v>2370</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>2473</v>
       </c>
@@ -39769,7 +39784,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="17" t="s">
         <v>212</v>
       </c>
@@ -39790,7 +39805,7 @@
         <v>2522</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>212</v>
       </c>
@@ -39811,7 +39826,7 @@
         <v>2504</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="17" t="s">
         <v>212</v>
       </c>
@@ -39832,7 +39847,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>212</v>
       </c>
@@ -39853,7 +39868,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>322</v>
       </c>
@@ -39874,7 +39889,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>2625</v>
       </c>
@@ -39895,7 +39910,7 @@
         <v>2696</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="17" t="s">
         <v>2625</v>
       </c>
@@ -39916,7 +39931,7 @@
         <v>2657</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>2625</v>
       </c>
@@ -39958,7 +39973,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>262</v>
       </c>
@@ -39979,7 +39994,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>2843</v>
       </c>
@@ -40000,7 +40015,7 @@
         <v>2878</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="17" t="s">
         <v>2843</v>
       </c>
@@ -40021,7 +40036,7 @@
         <v>2858</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>2843</v>
       </c>
@@ -40063,7 +40078,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>267</v>
       </c>
@@ -40084,7 +40099,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>3077</v>
       </c>
@@ -40105,7 +40120,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>3077</v>
       </c>
@@ -40147,7 +40162,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>227</v>
       </c>
@@ -40168,7 +40183,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>311</v>
       </c>
@@ -40189,7 +40204,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>217</v>
       </c>
@@ -40210,7 +40225,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="17" t="s">
         <v>257</v>
       </c>
@@ -40232,7 +40247,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G230"/>
+  <autoFilter ref="A1:G230">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="舆情特征分析"/>
+        <filter val="舆情特征分析 舆情演化分析"/>
+        <filter val="舆情特征分析 舆情引导对策"/>
+        <filter val="舆情特征分析 舆情应对方法"/>
+        <filter val="舆情特征分析 舆情预测"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>